<commit_message>
Update bot to calculate value to convert
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -397,45 +397,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v xml:space="preserve">Moeda Base: </v>
+        <v xml:space="preserve">Dia da cotação: </v>
       </c>
       <c r="B1" t="str">
-        <v>dolar</v>
+        <v>Tue May 21 2024 14:51:26 GMT-0400 (Amazon Standard Time)</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve">Moeda Desejada: </v>
+        <v xml:space="preserve">Cotação dolar: </v>
       </c>
       <c r="B2" t="str">
-        <v>real</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve">Resultado: </v>
+        <v xml:space="preserve">Cotação real: </v>
       </c>
       <c r="B3" t="str">
-        <v>1 dolar = 5.11 real</v>
+        <v>5.12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve">100 dolar convertido: </v>
+      </c>
+      <c r="B4" t="str">
+        <v>512 em real</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>